<commit_message>
Refactor move strategy, implement mobs
</commit_message>
<xml_diff>
--- a/game/data/world/map2.xlsx
+++ b/game/data/world/map2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\FunnyThings\gameproj\rpg-simulation\game\data\world\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41683039-146D-4B29-A523-F25F4BEF14D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B05368-9950-4BEF-8833-C434AA92213F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="13">
   <si>
     <t>battlefield</t>
   </si>
@@ -492,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA23"/>
+  <dimension ref="A1:AA26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE20" sqref="AE20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1275,8 +1275,8 @@
       <c r="I10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>8</v>
+      <c r="J10" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>4</v>
@@ -1302,8 +1302,8 @@
       <c r="R10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="S10" s="5" t="s">
-        <v>6</v>
+      <c r="S10" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="T10" s="5" t="s">
         <v>6</v>
@@ -1337,29 +1337,29 @@
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>8</v>
+      <c r="C11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>8</v>
+      <c r="G11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>4</v>
@@ -1385,8 +1385,8 @@
       <c r="R11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="S11" s="5" t="s">
-        <v>6</v>
+      <c r="S11" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="T11" s="5" t="s">
         <v>6</v>
@@ -1420,29 +1420,29 @@
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>8</v>
+      <c r="C12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>8</v>
+      <c r="G12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>4</v>
@@ -1468,8 +1468,8 @@
       <c r="R12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="S12" s="5" t="s">
-        <v>6</v>
+      <c r="S12" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="T12" s="5" t="s">
         <v>6</v>
@@ -1503,29 +1503,29 @@
       <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>8</v>
+      <c r="C13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>8</v>
+      <c r="G13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>4</v>
@@ -1551,8 +1551,8 @@
       <c r="R13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="S13" s="5" t="s">
-        <v>6</v>
+      <c r="S13" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="T13" s="5" t="s">
         <v>6</v>
@@ -1586,14 +1586,14 @@
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>8</v>
+      <c r="C14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>8</v>
@@ -1607,8 +1607,8 @@
       <c r="I14" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>8</v>
+      <c r="J14" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>4</v>
@@ -1616,17 +1616,17 @@
       <c r="L14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="M14" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="N14" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="O14" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="P14" s="8" t="s">
-        <v>0</v>
+      <c r="M14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="Q14" s="4" t="s">
         <v>5</v>
@@ -1634,8 +1634,8 @@
       <c r="R14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="S14" s="5" t="s">
-        <v>6</v>
+      <c r="S14" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="T14" s="5" t="s">
         <v>6</v>
@@ -1643,14 +1643,14 @@
       <c r="U14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="V14" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="W14" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="X14" s="10" t="s">
-        <v>7</v>
+      <c r="V14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="X14" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="Y14" s="5" t="s">
         <v>6</v>
@@ -1669,11 +1669,11 @@
       <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>2</v>
+      <c r="C15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>8</v>
@@ -1681,17 +1681,17 @@
       <c r="F15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>8</v>
+      <c r="G15" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>4</v>
@@ -1717,8 +1717,8 @@
       <c r="R15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="S15" s="5" t="s">
-        <v>6</v>
+      <c r="S15" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="T15" s="5" t="s">
         <v>6</v>
@@ -1726,14 +1726,14 @@
       <c r="U15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="V15" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="W15" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="X15" s="10" t="s">
-        <v>7</v>
+      <c r="V15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="X15" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="Y15" s="5" t="s">
         <v>6</v>
@@ -1764,17 +1764,17 @@
       <c r="F16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>8</v>
+      <c r="G16" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>4</v>
@@ -1800,8 +1800,8 @@
       <c r="R16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="S16" s="5" t="s">
-        <v>6</v>
+      <c r="S16" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="T16" s="5" t="s">
         <v>6</v>
@@ -1809,14 +1809,14 @@
       <c r="U16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="V16" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="W16" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="X16" s="10" t="s">
-        <v>7</v>
+      <c r="V16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="X16" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="Y16" s="5" t="s">
         <v>6</v>
@@ -1838,26 +1838,26 @@
       <c r="C17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>8</v>
+      <c r="D17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>8</v>
+      <c r="G17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>4</v>
@@ -1883,8 +1883,8 @@
       <c r="R17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="S17" s="5" t="s">
-        <v>6</v>
+      <c r="S17" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="T17" s="5" t="s">
         <v>6</v>
@@ -1921,26 +1921,26 @@
       <c r="C18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>8</v>
+      <c r="D18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>4</v>
@@ -1966,8 +1966,8 @@
       <c r="R18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="S18" s="5" t="s">
-        <v>6</v>
+      <c r="S18" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="T18" s="5" t="s">
         <v>6</v>
@@ -2004,26 +2004,26 @@
       <c r="C19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>8</v>
+      <c r="D19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>4</v>
@@ -2031,17 +2031,17 @@
       <c r="L19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="M19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>9</v>
+      <c r="M19" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="N19" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="P19" s="8" t="s">
+        <v>0</v>
       </c>
       <c r="Q19" s="4" t="s">
         <v>5</v>
@@ -2049,8 +2049,8 @@
       <c r="R19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="S19" s="5" t="s">
-        <v>6</v>
+      <c r="S19" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="T19" s="5" t="s">
         <v>6</v>
@@ -2058,14 +2058,14 @@
       <c r="U19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="V19" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="W19" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="X19" s="5" t="s">
-        <v>6</v>
+      <c r="V19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="W19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="X19" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="Y19" s="5" t="s">
         <v>6</v>
@@ -2087,26 +2087,26 @@
       <c r="C20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>8</v>
+      <c r="D20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>4</v>
@@ -2114,17 +2114,17 @@
       <c r="L20" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="M20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>9</v>
+      <c r="M20" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="N20" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="O20" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="P20" s="8" t="s">
+        <v>0</v>
       </c>
       <c r="Q20" s="4" t="s">
         <v>5</v>
@@ -2132,8 +2132,8 @@
       <c r="R20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="S20" s="5" t="s">
-        <v>6</v>
+      <c r="S20" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="T20" s="5" t="s">
         <v>6</v>
@@ -2141,14 +2141,14 @@
       <c r="U20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="V20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="W20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="X20" s="5" t="s">
-        <v>6</v>
+      <c r="V20" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="W20" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="X20" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="Y20" s="5" t="s">
         <v>6</v>
@@ -2188,8 +2188,8 @@
       <c r="I21" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="J21" s="2" t="s">
-        <v>8</v>
+      <c r="J21" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="K21" s="3" t="s">
         <v>4</v>
@@ -2197,17 +2197,17 @@
       <c r="L21" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>9</v>
+      <c r="M21" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="N21" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="O21" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="P21" s="8" t="s">
+        <v>0</v>
       </c>
       <c r="Q21" s="4" t="s">
         <v>5</v>
@@ -2215,8 +2215,8 @@
       <c r="R21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="S21" s="5" t="s">
-        <v>6</v>
+      <c r="S21" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="T21" s="5" t="s">
         <v>6</v>
@@ -2224,14 +2224,14 @@
       <c r="U21" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="V21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="W21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="X21" s="5" t="s">
-        <v>6</v>
+      <c r="V21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="W21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="X21" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="Y21" s="5" t="s">
         <v>6</v>
@@ -2253,26 +2253,26 @@
       <c r="C22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>8</v>
+      <c r="D22" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>4</v>
@@ -2298,8 +2298,8 @@
       <c r="R22" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="S22" s="5" t="s">
-        <v>6</v>
+      <c r="S22" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="T22" s="5" t="s">
         <v>6</v>
@@ -2330,38 +2330,38 @@
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>9</v>
+      <c r="B23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>9</v>
@@ -2375,37 +2375,286 @@
       <c r="P23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Q23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="T23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="U23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="V23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="W23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="X23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z23" s="1" t="s">
-        <v>9</v>
+      <c r="Q23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="R23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="U23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="X23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z23" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="AA23" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="R24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="U24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="X24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA24" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="R25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="U25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="X25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA25" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="U26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="W26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="X26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA26" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>